<commit_message>
Working Version of Small E. coli Model
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4545" windowWidth="16275" windowHeight="3300" firstSheet="5" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="4545" windowWidth="16275" windowHeight="3300" firstSheet="6" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,17 @@
     <sheet name="Sheet3" sheetId="9" r:id="rId14"/>
     <sheet name="Sheet7" sheetId="11" r:id="rId15"/>
     <sheet name="N2m" sheetId="17" r:id="rId16"/>
-    <sheet name="EcoliCCM" sheetId="18" r:id="rId17"/>
+    <sheet name="ecoliccm" sheetId="18" r:id="rId17"/>
+    <sheet name="Sheet9" sheetId="19" r:id="rId18"/>
+    <sheet name="ecoliT1" sheetId="20" r:id="rId19"/>
+    <sheet name="Sheet11" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="1236">
   <si>
     <t>Name</t>
   </si>
@@ -3669,6 +3672,96 @@
   </si>
   <si>
     <t>accoa[e]</t>
+  </si>
+  <si>
+    <t>akg[c] &lt;==&gt; akg[e]</t>
+  </si>
+  <si>
+    <t>EX_akg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h2o[c] &lt;==&gt; h2o[e] </t>
+  </si>
+  <si>
+    <t>EX_accoa</t>
+  </si>
+  <si>
+    <t>accoa[c] &lt;==&gt; accoa[e]</t>
+  </si>
+  <si>
+    <t>EX_h</t>
+  </si>
+  <si>
+    <t>h[c] &lt;==&gt; h[e]</t>
+  </si>
+  <si>
+    <t>h[e]</t>
+  </si>
+  <si>
+    <t>dhap[c] &lt;==&gt; dhap[e]</t>
+  </si>
+  <si>
+    <t>EX_dhap</t>
+  </si>
+  <si>
+    <t>G3P_ex</t>
+  </si>
+  <si>
+    <t>[c] : g3p + nad + pi + adp &lt;==&gt; pep + h + nadh + atp + h2o</t>
+  </si>
+  <si>
+    <t>[c] : 59.8100 atp + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 59.8100 h2o + 3.5470 nad + 13.0279 nadph + 7.5496 pep + 2.8328 pyr ---&gt; Biomass + 59.8100 adp + 7.8660 akg + 59.8100 h + 3.5470 nadh + 13.0279 nadp + 59.8100 pi</t>
+  </si>
+  <si>
+    <t>4 h[c] + nadh[c] --&gt; 3 h[e] + nad[c]</t>
+  </si>
+  <si>
+    <t>pi[c] &lt;==&gt; pi[e]</t>
+  </si>
+  <si>
+    <t>pyr[c] &lt;==&gt; pyr[e]</t>
+  </si>
+  <si>
+    <t>EX_pep</t>
+  </si>
+  <si>
+    <t>pep[c] &lt;==&gt; pep[e]</t>
+  </si>
+  <si>
+    <t>dhap[e]</t>
+  </si>
+  <si>
+    <t>pi[e]</t>
+  </si>
+  <si>
+    <t>pep[e]</t>
+  </si>
+  <si>
+    <t>pyr[e]</t>
+  </si>
+  <si>
+    <t>h2o[c] &lt;==&gt; h2o[e]</t>
+  </si>
+  <si>
+    <t>akg[e]</t>
+  </si>
+  <si>
+    <t>0.432,6000</t>
+  </si>
+  <si>
+    <t>[c] : fdp &lt;==&gt; g3p</t>
+  </si>
+  <si>
+    <t>[c] : g3p + pi + adp &lt;==&gt; pep + atp</t>
+  </si>
+  <si>
+    <t>EX_pi</t>
+  </si>
+  <si>
+    <t>EX_pyr</t>
+  </si>
+  <si>
+    <t>[c] : 59.8001 atp + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 7.5496 pep + 2.8328 pyr ---&gt; Biomass + 59.8001 adp + 59.8001 pi + 59.8001 h</t>
   </si>
 </sst>
 </file>
@@ -3771,7 +3864,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -3804,6 +3897,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -6196,7 +6290,7 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9274,17 +9368,17 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" customWidth="1"/>
     <col min="15" max="15" width="13.85546875" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
@@ -9341,25 +9435,29 @@
     </row>
     <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="B2" s="14"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="31">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23">
+        <v>0</v>
+      </c>
       <c r="G2" s="29">
-        <v>-10</v>
+        <v>29.175799999999999</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>1156</v>
+        <v>1208</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="O2" s="28">
         <v>0</v>
       </c>
       <c r="P2" s="28">
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9380,13 +9478,13 @@
         <v>1155</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>1023</v>
+        <v>1132</v>
       </c>
       <c r="O3" s="28">
-        <v>0.128</v>
+        <v>0</v>
       </c>
       <c r="P3" s="28">
-        <v>0.128</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9407,7 +9505,7 @@
         <v>891</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>1096</v>
+        <v>1133</v>
       </c>
       <c r="O4" s="28">
         <v>0</v>
@@ -9434,10 +9532,10 @@
         <v>889</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>1024</v>
+        <v>1015</v>
       </c>
       <c r="O5" s="28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P5" s="28">
         <v>0.5</v>
@@ -9461,13 +9559,13 @@
         <v>872</v>
       </c>
       <c r="N6" s="28" t="s">
-        <v>1027</v>
+        <v>1205</v>
       </c>
       <c r="O6" s="28">
-        <v>2.0799999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="P6" s="28">
-        <v>2.0799999999999998E-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9488,13 +9586,13 @@
         <v>871</v>
       </c>
       <c r="N7" s="28" t="s">
-        <v>1028</v>
+        <v>1036</v>
       </c>
       <c r="O7" s="28">
-        <v>0.47299999999999998</v>
+        <v>0</v>
       </c>
       <c r="P7" s="28">
-        <v>0.47299999999999998</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9515,13 +9613,13 @@
         <v>1154</v>
       </c>
       <c r="N8" s="28" t="s">
-        <v>1138</v>
+        <v>1034</v>
       </c>
       <c r="O8" s="28">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P8" s="28">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9542,13 +9640,13 @@
         <v>1199</v>
       </c>
       <c r="N9" s="28" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="O9" s="28">
-        <v>0</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="P9" s="28">
-        <v>0.05</v>
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9569,13 +9667,13 @@
         <v>1200</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>1026</v>
+        <v>1037</v>
       </c>
       <c r="O10" s="28">
         <v>0</v>
       </c>
       <c r="P10" s="28">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9596,13 +9694,13 @@
         <v>870</v>
       </c>
       <c r="N11" s="28" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="O11" s="28">
-        <v>1.37</v>
+        <v>0</v>
       </c>
       <c r="P11" s="28">
-        <v>1.37</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9623,13 +9721,13 @@
         <v>1169</v>
       </c>
       <c r="N12" s="28" t="s">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="O12" s="28">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="P12" s="28">
-        <v>0.5</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -9650,7 +9748,7 @@
         <v>1170</v>
       </c>
       <c r="N13" s="28" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="O13" s="28">
         <v>0</v>
@@ -9677,7 +9775,7 @@
         <v>895</v>
       </c>
       <c r="N14" s="28" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="O14" s="28">
         <v>0</v>
@@ -9704,7 +9802,7 @@
         <v>978</v>
       </c>
       <c r="N15" s="28" t="s">
-        <v>1036</v>
+        <v>1136</v>
       </c>
       <c r="O15" s="28">
         <v>0</v>
@@ -9731,7 +9829,7 @@
         <v>888</v>
       </c>
       <c r="N16" s="28" t="s">
-        <v>1034</v>
+        <v>1135</v>
       </c>
       <c r="O16" s="28">
         <v>0</v>
@@ -9758,7 +9856,7 @@
         <v>984</v>
       </c>
       <c r="N17" s="28" t="s">
-        <v>1136</v>
+        <v>1046</v>
       </c>
       <c r="O17" s="28">
         <v>0</v>
@@ -9785,7 +9883,7 @@
         <v>980</v>
       </c>
       <c r="N18" s="28" t="s">
-        <v>1047</v>
+        <v>1096</v>
       </c>
       <c r="O18" s="28">
         <v>0</v>
@@ -9812,13 +9910,13 @@
         <v>885</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>1135</v>
+        <v>1157</v>
       </c>
       <c r="O19" s="28">
         <v>0</v>
       </c>
       <c r="P19" s="28">
-        <v>0.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -9828,8 +9926,12 @@
       <c r="B20" s="14"/>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="28"/>
+      <c r="E20" s="31">
+        <v>0</v>
+      </c>
+      <c r="F20" s="23">
+        <v>0</v>
+      </c>
       <c r="G20" s="29">
         <v>0.87390000000000001</v>
       </c>
@@ -9837,7 +9939,7 @@
         <v>1201</v>
       </c>
       <c r="N20" t="s">
-        <v>1133</v>
+        <v>1047</v>
       </c>
       <c r="O20" s="28">
         <v>0</v>
@@ -9847,55 +9949,837 @@
       </c>
     </row>
     <row r="21" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E21" s="31">
+        <v>0</v>
+      </c>
+      <c r="F21" s="23">
+        <v>0</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>1206</v>
+      </c>
       <c r="N21" s="28" t="s">
+        <v>1213</v>
+      </c>
+      <c r="O21" s="28">
+        <v>0</v>
+      </c>
+      <c r="P21" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E22" s="31">
+        <v>0</v>
+      </c>
+      <c r="F22" s="23">
+        <v>0</v>
+      </c>
+      <c r="G22" s="29">
+        <v>0</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>1210</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1202</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E23" s="31">
+        <v>0</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="29">
+        <v>0</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>1212</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1203</v>
+      </c>
+      <c r="O23" s="28">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E24" s="31">
+        <v>0</v>
+      </c>
+      <c r="F24" s="23">
+        <v>0</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>1214</v>
+      </c>
+      <c r="N24" t="s">
+        <v>1029</v>
+      </c>
+      <c r="O24" s="28">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>1028</v>
+      </c>
+      <c r="O25" s="28">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="P25">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>1027</v>
+      </c>
+      <c r="O26" s="28">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="P26">
+        <v>2.0799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O27" s="28">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>1173</v>
+      </c>
+      <c r="O28" s="28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>1204</v>
+      </c>
+      <c r="O29" s="28">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>1024</v>
+      </c>
+      <c r="O30" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="P30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>1138</v>
+      </c>
+      <c r="O31" s="28">
+        <v>1E-4</v>
+      </c>
+      <c r="P31">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>1023</v>
+      </c>
+      <c r="O32" s="28">
+        <v>0.128</v>
+      </c>
+      <c r="P32">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>1197</v>
+      </c>
+      <c r="O33" s="28">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>1198</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="N2:P34">
+    <sortCondition ref="N2:N34"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>986</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>838</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>944</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="E2" s="31">
+        <v>4581156.7432856048</v>
+      </c>
+      <c r="F2" s="23">
+        <v>-9.1</v>
+      </c>
+      <c r="G2" s="29">
+        <v>10</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>1155</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>1157</v>
+      </c>
+      <c r="O2" s="28">
+        <v>1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="E3" s="31">
+        <v>3.8510595392951203</v>
+      </c>
+      <c r="F3" s="23">
+        <v>-0.8</v>
+      </c>
+      <c r="G3" s="29">
+        <v>4.8609</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>1230</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>1046</v>
+      </c>
+      <c r="O3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="E4" s="31">
+        <v>604.65285404763836</v>
+      </c>
+      <c r="F4" s="23">
+        <v>-3.8</v>
+      </c>
+      <c r="G4" s="29">
+        <v>7.4774000000000003</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>889</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>1024</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0.184</v>
+      </c>
+      <c r="P4" s="28">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="E5" s="31">
+        <v>8.4275973191444799E-4</v>
+      </c>
+      <c r="F5" s="23">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="29">
+        <v>7.4774000000000003</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>871</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>1023</v>
+      </c>
+      <c r="O5" s="28">
+        <v>0.128</v>
+      </c>
+      <c r="P5" s="28">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29">
+        <v>0</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>1214</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O6" s="28">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="P6" s="28">
+        <v>4.3900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="E7" s="31">
+        <v>1.1835797581124567</v>
+      </c>
+      <c r="F7" s="23">
+        <v>-0.1</v>
+      </c>
+      <c r="G7" s="29">
+        <v>16.023499999999999</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>1217</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>1136</v>
+      </c>
+      <c r="O7" s="28">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="P7" s="28">
+        <v>2.5899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="E8" s="31">
+        <v>7576.5072679615205</v>
+      </c>
+      <c r="F8" s="23">
+        <v>-5.3</v>
+      </c>
+      <c r="G8" s="29">
+        <v>1.7582</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>1040</v>
+      </c>
+      <c r="O8" s="28">
+        <v>0.126</v>
+      </c>
+      <c r="P8" s="28">
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="E9" s="31">
+        <v>7.5573641589575944</v>
+      </c>
+      <c r="F9" s="23">
+        <v>-1.2</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>978</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>1224</v>
+      </c>
+      <c r="O9" s="28">
+        <v>0</v>
+      </c>
+      <c r="P9" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>849</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>1218</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1135</v>
+      </c>
+      <c r="O10">
+        <v>0.02</v>
+      </c>
+      <c r="P10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>974</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="E11" s="31">
+        <v>0.60312511374657485</v>
+      </c>
+      <c r="F11" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>980</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>1029</v>
+      </c>
+      <c r="O11" s="28">
+        <v>5.3499999999999997E-3</v>
+      </c>
+      <c r="P11" s="28">
+        <v>5.3499999999999997E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>959</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="E12" s="26">
+        <v>5449668303594.3379</v>
+      </c>
+      <c r="F12" s="21">
+        <v>-17.399999999999999</v>
+      </c>
+      <c r="G12" s="29">
+        <v>38.534599999999998</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>1219</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>1028</v>
+      </c>
+      <c r="O12" s="28">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="P12" s="28">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>960</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="E13" s="31">
+        <v>1.6580307753859953</v>
+      </c>
+      <c r="F13" s="23">
+        <v>-0.3</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>885</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>1036</v>
+      </c>
+      <c r="O13" s="28">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="P13" s="28">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0</v>
+      </c>
+      <c r="F14" s="23">
+        <v>0</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>1206</v>
+      </c>
+      <c r="N14" s="28" t="s">
         <v>1033</v>
       </c>
-      <c r="O21" s="28">
+      <c r="O14" s="28">
         <v>9.6300000000000008</v>
       </c>
-      <c r="P21" s="28">
+      <c r="P14" s="28">
         <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>935</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="E15" s="31">
+        <v>0</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0</v>
+      </c>
+      <c r="G15" s="29">
+        <v>-3.2149000000000001</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>1220</v>
+      </c>
+      <c r="N15" s="28" t="s">
+        <v>1138</v>
+      </c>
+      <c r="O15" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P15" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>936</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="E16" s="31">
+        <v>0</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>1221</v>
+      </c>
+      <c r="N16" s="28" t="s">
+        <v>1225</v>
+      </c>
+      <c r="O16" s="28">
+        <v>0</v>
+      </c>
+      <c r="P16" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>929</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="E17" s="31">
+        <v>0</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0</v>
+      </c>
+      <c r="G17" s="29">
+        <v>17.530899999999999</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>1212</v>
+      </c>
+      <c r="N17" s="28" t="s">
+        <v>1027</v>
+      </c>
+      <c r="O17" s="28">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="P17" s="28">
+        <v>2.0799999999999998E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>930</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="E18" s="31">
+        <v>0</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0</v>
+      </c>
+      <c r="G18" s="29">
+        <v>29.175799999999999</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>1228</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O18" s="28">
+        <v>0.121</v>
+      </c>
+      <c r="P18" s="28">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E19" s="31">
+        <v>0</v>
+      </c>
+      <c r="F19" s="23">
+        <v>0</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>1223</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1202</v>
+      </c>
+      <c r="O19">
+        <v>50</v>
+      </c>
+      <c r="P19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="O20">
+        <v>50</v>
+      </c>
+      <c r="P20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>1047</v>
+      </c>
+      <c r="O21">
+        <v>1E-4</v>
+      </c>
+      <c r="P21">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
-        <v>1132</v>
+        <v>1213</v>
       </c>
       <c r="O22">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P22">
-        <v>0.5</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N23" t="s">
-        <v>1153</v>
-      </c>
-      <c r="O23" s="28">
+        <v>1226</v>
+      </c>
+      <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N24" t="s">
-        <v>1173</v>
-      </c>
-      <c r="O24" s="28">
+        <v>1227</v>
+      </c>
+      <c r="O24">
         <v>0</v>
       </c>
       <c r="P24">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N25" t="s">
-        <v>1037</v>
-      </c>
-      <c r="O25" s="28">
-        <v>0</v>
+        <v>1035</v>
+      </c>
+      <c r="O25">
+        <v>0.1</v>
       </c>
       <c r="P25">
         <v>0.5</v>
@@ -9903,95 +10787,367 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N26" t="s">
-        <v>1038</v>
-      </c>
-      <c r="O26" s="28">
+        <v>1229</v>
+      </c>
+      <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N27" t="s">
-        <v>1202</v>
-      </c>
-      <c r="O27" s="28">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N28" t="s">
-        <v>1203</v>
-      </c>
-      <c r="O28" s="28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N29" t="s">
-        <v>1015</v>
-      </c>
-      <c r="O29" s="28">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N30" t="s">
-        <v>1204</v>
-      </c>
-      <c r="O30" s="28">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N31" t="s">
-        <v>1205</v>
-      </c>
-      <c r="O31" s="28">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N32" t="s">
-        <v>1197</v>
-      </c>
-      <c r="O32" s="28">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N33" t="s">
-        <v>1198</v>
-      </c>
-      <c r="O33" s="28">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>985</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>986</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>861</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>838</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>944</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="E2" s="31">
+        <v>4581156.7432856048</v>
+      </c>
+      <c r="F2" s="23">
+        <v>-9.1</v>
+      </c>
+      <c r="G2" s="29">
+        <v>10</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>1155</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>1157</v>
+      </c>
+      <c r="O2" s="28">
+        <v>1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="E3" s="31">
+        <v>3.8510595392951203</v>
+      </c>
+      <c r="F3" s="23">
+        <v>-0.8</v>
+      </c>
+      <c r="G3" s="29">
+        <v>4.8609</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>1046</v>
+      </c>
+      <c r="O3" s="28">
+        <v>1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="E4" s="31">
+        <v>604.65285404763836</v>
+      </c>
+      <c r="F4" s="23">
+        <v>-3.8</v>
+      </c>
+      <c r="G4" s="29">
+        <v>7.4774000000000003</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>889</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>1024</v>
+      </c>
+      <c r="O4" s="28">
+        <v>1</v>
+      </c>
+      <c r="P4" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="E5" s="31">
+        <v>8.4275973191444799E-4</v>
+      </c>
+      <c r="F5" s="23">
+        <v>4.2</v>
+      </c>
+      <c r="G5" s="29">
+        <v>7.4774000000000003</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>1231</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>1023</v>
+      </c>
+      <c r="O5" s="28">
+        <v>1</v>
+      </c>
+      <c r="P5" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="E6" s="31">
+        <v>1.1835797581124567</v>
+      </c>
+      <c r="F6" s="23">
+        <v>-0.1</v>
+      </c>
+      <c r="G6" s="29">
+        <v>16.023499999999999</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>1232</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O6" s="28">
+        <v>1</v>
+      </c>
+      <c r="P6" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="E7" s="31">
+        <v>7576.5072679615205</v>
+      </c>
+      <c r="F7" s="23">
+        <v>-5.3</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1.7582</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>895</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>1136</v>
+      </c>
+      <c r="O7" s="28">
+        <v>1</v>
+      </c>
+      <c r="P7" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>849</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>1235</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="O8" s="28">
+        <v>1</v>
+      </c>
+      <c r="P8" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>1212</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>1036</v>
+      </c>
+      <c r="O9" s="28">
+        <v>1</v>
+      </c>
+      <c r="P9" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>1220</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>1033</v>
+      </c>
+      <c r="O10" s="28">
+        <v>1</v>
+      </c>
+      <c r="P10" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>1221</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>1138</v>
+      </c>
+      <c r="O11" s="28">
+        <v>1</v>
+      </c>
+      <c r="P11" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>1047</v>
+      </c>
+      <c r="O12">
+        <v>1E-4</v>
+      </c>
+      <c r="P12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>1225</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>1213</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>1227</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10206,6 +11362,142 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B1" s="28">
+        <v>1</v>
+      </c>
+      <c r="C1" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0.184</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0.128</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B5" s="28">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="C5" s="28">
+        <v>4.3900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B6" s="28">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="C6" s="28">
+        <v>2.5899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="28">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B9" s="28">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="C9" s="28">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B11" s="28">
+        <v>1E-4</v>
+      </c>
+      <c r="C11" s="28">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>
@@ -54503,8 +55795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Addition of flux time course + Sorted scale-up issues
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2339" uniqueCount="1238">
   <si>
     <t>Name</t>
   </si>
@@ -3762,6 +3762,12 @@
   </si>
   <si>
     <t>[c] : 59.8001 atp + 0.0709 f6p + 0.1290 g3p + 0.2050 g6p + 7.5496 pep + 2.8328 pyr ---&gt; Biomass + 59.8001 adp + 59.8001 pi + 59.8001 h</t>
+  </si>
+  <si>
+    <t>glc[c] ---&gt; g6p[c]</t>
+  </si>
+  <si>
+    <t>glc[e] ---&gt; glc[c]</t>
   </si>
 </sst>
 </file>
@@ -10804,10 +10810,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10881,7 +10887,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>1155</v>
+        <v>1237</v>
       </c>
       <c r="N2" s="28" t="s">
         <v>1157</v>
@@ -10895,20 +10901,16 @@
     </row>
     <row r="3" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>587</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="E3" s="31">
-        <v>3.8510595392951203</v>
-      </c>
-      <c r="F3" s="23">
-        <v>-0.8</v>
-      </c>
-      <c r="G3" s="29">
-        <v>4.8609</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>891</v>
+        <v>944</v>
+      </c>
+      <c r="F3" s="28">
+        <v>-9.1</v>
+      </c>
+      <c r="G3" s="28">
+        <v>10</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>1236</v>
       </c>
       <c r="N3" s="28" t="s">
         <v>1046</v>
@@ -10922,20 +10924,20 @@
     </row>
     <row r="4" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B4" s="14"/>
       <c r="E4" s="31">
-        <v>604.65285404763836</v>
+        <v>3.8510595392951203</v>
       </c>
       <c r="F4" s="23">
-        <v>-3.8</v>
+        <v>-0.8</v>
       </c>
       <c r="G4" s="29">
-        <v>7.4774000000000003</v>
+        <v>4.8609</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="N4" s="28" t="s">
         <v>1024</v>
@@ -10949,20 +10951,20 @@
     </row>
     <row r="5" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B5" s="14"/>
       <c r="E5" s="31">
-        <v>8.4275973191444799E-4</v>
+        <v>604.65285404763836</v>
       </c>
       <c r="F5" s="23">
-        <v>4.2</v>
+        <v>-3.8</v>
       </c>
       <c r="G5" s="29">
         <v>7.4774000000000003</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>1231</v>
+        <v>889</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>1023</v>
@@ -10976,20 +10978,20 @@
     </row>
     <row r="6" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>1216</v>
+        <v>589</v>
       </c>
       <c r="B6" s="14"/>
       <c r="E6" s="31">
-        <v>1.1835797581124567</v>
+        <v>8.4275973191444799E-4</v>
       </c>
       <c r="F6" s="23">
-        <v>-0.1</v>
+        <v>4.2</v>
       </c>
       <c r="G6" s="29">
-        <v>16.023499999999999</v>
+        <v>7.4774000000000003</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>1042</v>
@@ -11003,20 +11005,20 @@
     </row>
     <row r="7" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>595</v>
+        <v>1216</v>
       </c>
       <c r="B7" s="14"/>
       <c r="E7" s="31">
-        <v>7576.5072679615205</v>
+        <v>1.1835797581124567</v>
       </c>
       <c r="F7" s="23">
-        <v>-5.3</v>
+        <v>-0.1</v>
       </c>
       <c r="G7" s="29">
-        <v>1.7582</v>
+        <v>16.023499999999999</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>895</v>
+        <v>1232</v>
       </c>
       <c r="N7" s="28" t="s">
         <v>1136</v>
@@ -11030,16 +11032,20 @@
     </row>
     <row r="8" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>849</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="B8" s="14"/>
       <c r="E8" s="31">
-        <v>0</v>
+        <v>7576.5072679615205</v>
       </c>
       <c r="F8" s="23">
-        <v>0</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>1235</v>
+        <v>-5.3</v>
+      </c>
+      <c r="G8" s="29">
+        <v>1.7582</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>895</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>1135</v>
@@ -11053,10 +11059,20 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>1211</v>
-      </c>
+        <v>849</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="31">
+        <v>0</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0</v>
+      </c>
+      <c r="G9" s="28"/>
       <c r="H9" s="32" t="s">
-        <v>1212</v>
+        <v>1235</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>1036</v>
@@ -11070,10 +11086,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>1233</v>
+        <v>1211</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>1220</v>
+        <v>1212</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>1033</v>
@@ -11087,10 +11103,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="N11" s="28" t="s">
         <v>1138</v>
@@ -11103,14 +11119,20 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>1221</v>
+      </c>
       <c r="N12" t="s">
         <v>1047</v>
       </c>
       <c r="O12">
-        <v>1E-4</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>1E-4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -11132,7 +11154,7 @@
         <v>1</v>
       </c>
       <c r="P14">
-        <v>2E-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -11144,6 +11166,17 @@
       </c>
       <c r="P15">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>1096</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update July 02 2015
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -23,14 +23,15 @@
     <sheet name="Sheet3" sheetId="9" r:id="rId14"/>
     <sheet name="Sheet7" sheetId="11" r:id="rId15"/>
     <sheet name="N2m" sheetId="17" r:id="rId16"/>
-    <sheet name="EcoliCCM" sheetId="18" r:id="rId17"/>
+    <sheet name="N3m" sheetId="19" r:id="rId17"/>
+    <sheet name="EcoliCCM" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="1241">
   <si>
     <t>Name</t>
   </si>
@@ -3699,6 +3700,81 @@
   </si>
   <si>
     <t>20 B[c] ---&gt; Biomass</t>
+  </si>
+  <si>
+    <t>&lt;==&gt; S[e]</t>
+  </si>
+  <si>
+    <t>S[e] ---&gt; S[c]</t>
+  </si>
+  <si>
+    <t>[c] : S ---&gt; B</t>
+  </si>
+  <si>
+    <t>[c] : S ---&gt; A</t>
+  </si>
+  <si>
+    <t>[c] : S ---&gt; M</t>
+  </si>
+  <si>
+    <t>[c] : S ---&gt; P</t>
+  </si>
+  <si>
+    <t>[c] : M ---&gt; N</t>
+  </si>
+  <si>
+    <t>[c] : M + N ---&gt; A + K</t>
+  </si>
+  <si>
+    <t>[c] : N ---&gt; K</t>
+  </si>
+  <si>
+    <t>[c] : K ---&gt; B + P</t>
+  </si>
+  <si>
+    <t>B[c] ---&gt; B[e]</t>
+  </si>
+  <si>
+    <t>A[c] ---&gt; A[e]</t>
+  </si>
+  <si>
+    <t>B[e] ---&gt;</t>
+  </si>
+  <si>
+    <t>A[e] ---&gt;</t>
+  </si>
+  <si>
+    <t>biomass[c] ---&gt;</t>
+  </si>
+  <si>
+    <t>S[c]</t>
+  </si>
+  <si>
+    <t>M[c]</t>
+  </si>
+  <si>
+    <t>N[c]</t>
+  </si>
+  <si>
+    <t>K[c]</t>
+  </si>
+  <si>
+    <t>S[e]</t>
+  </si>
+  <si>
+    <t>B[e]</t>
+  </si>
+  <si>
+    <t>P[e]</t>
+  </si>
+  <si>
+    <t>Bex</t>
+  </si>
+  <si>
+    <t>exS</t>
+  </si>
+  <si>
+    <t>[c] : 10 M  + 5 N ---&gt; biomass</t>
   </si>
 </sst>
 </file>
@@ -8881,7 +8957,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8975,7 +9051,7 @@
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28">
-        <v>-0.5</v>
+        <v>-8</v>
       </c>
       <c r="G3" s="28">
         <v>20</v>
@@ -9013,7 +9089,7 @@
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28">
-        <v>-0.5</v>
+        <v>-8</v>
       </c>
       <c r="G4" s="28">
         <v>5</v>
@@ -9051,7 +9127,7 @@
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28">
-        <v>-0.5</v>
+        <v>-8</v>
       </c>
       <c r="G5" s="28">
         <v>10</v>
@@ -9089,7 +9165,7 @@
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="28">
         <v>5</v>
@@ -9127,7 +9203,7 @@
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28">
-        <v>-0.5</v>
+        <v>-8</v>
       </c>
       <c r="G7" s="28">
         <v>2.5</v>
@@ -9165,7 +9241,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28">
-        <v>-0.5</v>
+        <v>-8</v>
       </c>
       <c r="G8" s="28">
         <v>5</v>
@@ -9197,7 +9273,7 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="28">
         <v>2.5</v>
@@ -9387,6 +9463,591 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>818</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>828</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
+        <v>1216</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="s">
+        <v>1193</v>
+      </c>
+      <c r="O2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G3" s="28">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28" t="s">
+        <v>1231</v>
+      </c>
+      <c r="O3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G4" s="28">
+        <v>5</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>1218</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>764</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G5" s="28">
+        <v>10</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="O5" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B6" s="28">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
+        <v>0</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G6" s="28">
+        <v>5</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O6" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P6" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <v>0</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G7" s="28">
+        <v>5</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>1221</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
+        <v>1233</v>
+      </c>
+      <c r="O7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G8" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>1222</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28" t="s">
+        <v>1234</v>
+      </c>
+      <c r="O8" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P8" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G9" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>1223</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="O9" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P9" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28" t="s">
+        <v>1236</v>
+      </c>
+      <c r="O10" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P10" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28" t="s">
+        <v>1237</v>
+      </c>
+      <c r="O11" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P11" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28" t="s">
+        <v>1226</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>849</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
+        <v>1228</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Parallel Monte Carlo Simulation of Ensmeble of Models
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4605" windowWidth="16275" windowHeight="3240" firstSheet="5" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="4605" windowWidth="16275" windowHeight="3240" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2260" uniqueCount="1241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="1238">
   <si>
     <t>Name</t>
   </si>
@@ -3630,9 +3630,6 @@
     <t>E[c] ---&gt; E[e]</t>
   </si>
   <si>
-    <t>D[c] ---&gt; D[e]</t>
-  </si>
-  <si>
     <t>A[c]</t>
   </si>
   <si>
@@ -3672,16 +3669,10 @@
     <t>Eex</t>
   </si>
   <si>
-    <t>Dex</t>
-  </si>
-  <si>
     <t>P[e] ---&gt;</t>
   </si>
   <si>
     <t>E[e] ---&gt;</t>
-  </si>
-  <si>
-    <t>D[e] ---&gt;</t>
   </si>
   <si>
     <t>BiomassEX</t>
@@ -8954,10 +8945,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9018,10 +9009,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="H2" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -9029,7 +9020,7 @@
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" s="28" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="O2" s="28">
         <v>0.1</v>
@@ -9057,7 +9048,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -9165,10 +9156,10 @@
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="28">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>1189</v>
@@ -9209,7 +9200,7 @@
         <v>2.5</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -9273,7 +9264,7 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G9" s="28">
         <v>2.5</v>
@@ -9344,7 +9335,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1062</v>
+        <v>849</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -9356,30 +9347,32 @@
         <v>-0.5</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>0.33</v>
       </c>
       <c r="H12" t="s">
-        <v>1192</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>849</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+        <v>1203</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28">
         <v>-0.5</v>
       </c>
       <c r="G13">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>1215</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -9401,60 +9394,23 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B15" s="28">
-        <v>0</v>
-      </c>
-      <c r="C15" s="28">
-        <v>0</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
+        <v>1207</v>
       </c>
       <c r="H15" t="s">
-        <v>1208</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B16" s="28">
-        <v>0</v>
-      </c>
-      <c r="C16" s="28">
-        <v>0</v>
-      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1214</v>
-      </c>
+      <c r="F16" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9466,8 +9422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9524,7 +9480,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -9533,7 +9489,7 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
       <c r="H2" s="28" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -9541,7 +9497,7 @@
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" s="28" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="O2" s="28">
         <v>0.1</v>
@@ -9569,7 +9525,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -9577,7 +9533,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
       <c r="N3" s="28" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="O3" s="28">
         <v>0.1</v>
@@ -9605,7 +9561,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -9641,15 +9597,17 @@
         <v>10</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="J5" s="28" t="s">
+        <v>1125</v>
+      </c>
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="O5" s="28">
         <v>0.1</v>
@@ -9677,7 +9635,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -9713,7 +9671,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -9721,7 +9679,7 @@
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="O7" s="28">
         <v>0.1</v>
@@ -9743,13 +9701,13 @@
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="28">
         <v>2.5</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -9757,7 +9715,7 @@
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="O8" s="28">
         <v>0.1</v>
@@ -9779,13 +9737,13 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="28">
         <v>2.5</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -9793,7 +9751,7 @@
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="O9" s="28">
         <v>0.1</v>
@@ -9821,7 +9779,7 @@
         <v>2.5</v>
       </c>
       <c r="H10" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -9829,7 +9787,7 @@
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="O10" s="28">
         <v>0.1</v>
@@ -9857,7 +9815,7 @@
         <v>2.5</v>
       </c>
       <c r="H11" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
@@ -9865,7 +9823,7 @@
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="O11" s="28">
         <v>0.1</v>
@@ -9907,7 +9865,7 @@
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
@@ -9929,7 +9887,7 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -9959,7 +9917,7 @@
         <v>0.33</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -9972,7 +9930,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -9981,7 +9939,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
@@ -9994,7 +9952,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -10003,7 +9961,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
@@ -10016,7 +9974,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -10025,12 +9983,12 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -10039,7 +9997,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -10314,7 +10272,7 @@
         <v>16.023499999999999</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>1029</v>
@@ -10341,7 +10299,7 @@
         <v>14.716100000000001</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>1026</v>
@@ -10609,7 +10567,7 @@
         <v>0.87390000000000001</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="N20" t="s">
         <v>1133</v>
@@ -10689,7 +10647,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N27" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="O27" s="28">
         <v>0</v>
@@ -10700,7 +10658,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="O28" s="28">
         <v>0</v>
@@ -10722,7 +10680,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="O30" s="28">
         <v>0</v>
@@ -10733,7 +10691,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="O31" s="28">
         <v>0</v>
@@ -10744,7 +10702,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="O32" s="28">
         <v>0</v>
@@ -10755,7 +10713,7 @@
     </row>
     <row r="33" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="O33" s="28">
         <v>0</v>
@@ -56852,7 +56810,7 @@
         <v>884</v>
       </c>
       <c r="N60" s="28" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="O60" s="28">
         <v>0</v>
@@ -56879,7 +56837,7 @@
         <v>1149</v>
       </c>
       <c r="N61" s="28" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="O61" s="28">
         <v>0</v>

</xml_diff>

<commit_message>
Modified TRNModel-Need changes to allow use with TRNModel
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4605" windowWidth="16275" windowHeight="3240" firstSheet="5" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" firstSheet="5" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sheet6" sheetId="10" r:id="rId13"/>
     <sheet name="Sheet3" sheetId="9" r:id="rId14"/>
     <sheet name="Sheet7" sheetId="11" r:id="rId15"/>
-    <sheet name="N2m" sheetId="17" r:id="rId16"/>
+    <sheet name="N2am" sheetId="17" r:id="rId16"/>
     <sheet name="N3m" sheetId="19" r:id="rId17"/>
     <sheet name="EcoliCCM" sheetId="18" r:id="rId18"/>
   </sheets>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="1240">
   <si>
     <t>Name</t>
   </si>
@@ -3621,9 +3621,6 @@
     <t>[c] : A ---&gt; B</t>
   </si>
   <si>
-    <t>[c] : A ---&gt; D</t>
-  </si>
-  <si>
     <t>P[c] ---&gt; P[e]</t>
   </si>
   <si>
@@ -3687,12 +3684,6 @@
     <t>&lt;==&gt; A[e]</t>
   </si>
   <si>
-    <t>Biomass ---&gt;</t>
-  </si>
-  <si>
-    <t>20 B[c] ---&gt; Biomass</t>
-  </si>
-  <si>
     <t>&lt;==&gt; S[e]</t>
   </si>
   <si>
@@ -3766,6 +3757,21 @@
   </si>
   <si>
     <t>[c] : 10 M  + 5 N ---&gt; biomass</t>
+  </si>
+  <si>
+    <t>[c] : D ---&gt; A</t>
+  </si>
+  <si>
+    <t>[c] : P + E ---&gt; C + D</t>
+  </si>
+  <si>
+    <t>20 B[c] ---&gt; Biomass[c]</t>
+  </si>
+  <si>
+    <t>Biomass[c] ---&gt;</t>
+  </si>
+  <si>
+    <t>EC_biomass</t>
   </si>
 </sst>
 </file>
@@ -8948,12 +8954,12 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
@@ -9010,10 +9016,10 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1208</v>
+      </c>
+      <c r="H2" t="s">
         <v>1209</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1210</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -9021,7 +9027,7 @@
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" s="28" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="O2" s="28">
         <v>0.1</v>
@@ -9049,7 +9055,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -9084,7 +9090,7 @@
         <v>-8</v>
       </c>
       <c r="G4" s="28">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>1187</v>
@@ -9122,7 +9128,7 @@
         <v>-8</v>
       </c>
       <c r="G5" s="28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>1188</v>
@@ -9154,18 +9160,16 @@
       <c r="C6" s="28">
         <v>0</v>
       </c>
-      <c r="D6" s="28">
-        <v>100</v>
-      </c>
+      <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>7</v>
+        <v>-8</v>
       </c>
       <c r="G6" s="28">
-        <v>2.5</v>
+        <v>40</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>1189</v>
+        <v>1235</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -9200,10 +9204,10 @@
         <v>-8</v>
       </c>
       <c r="G7" s="28">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -9238,7 +9242,7 @@
         <v>-8</v>
       </c>
       <c r="G8" s="28">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>1117</v>
@@ -9267,13 +9271,13 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>7</v>
+        <v>-8</v>
       </c>
       <c r="G9" s="28">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>1118</v>
+        <v>1236</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -9303,7 +9307,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -9333,12 +9337,12 @@
         <v>2.5</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>849</v>
+        <v>1239</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -9353,12 +9357,12 @@
         <v>0.33</v>
       </c>
       <c r="H12" t="s">
-        <v>1212</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B13" s="28">
         <v>0</v>
@@ -9375,12 +9379,12 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B14" s="28">
         <v>0</v>
@@ -9397,15 +9401,15 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="H15" t="s">
-        <v>1211</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -9426,7 +9430,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9483,7 +9487,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -9492,7 +9496,7 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
       <c r="H2" s="28" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
@@ -9500,7 +9504,7 @@
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" s="28" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="O2" s="28">
         <v>0.1</v>
@@ -9528,7 +9532,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -9536,7 +9540,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
       <c r="N3" s="28" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="O3" s="28">
         <v>0.1</v>
@@ -9561,10 +9565,10 @@
         <v>-0.5</v>
       </c>
       <c r="G4" s="28">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -9597,10 +9601,10 @@
         <v>-0.5</v>
       </c>
       <c r="G5" s="28">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="28" t="s">
@@ -9610,7 +9614,7 @@
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
       <c r="N5" s="28" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="O5" s="28">
         <v>0.1</v>
@@ -9635,10 +9639,10 @@
         <v>-0.5</v>
       </c>
       <c r="G6" s="28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -9674,7 +9678,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -9682,7 +9686,7 @@
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="O7" s="28">
         <v>0.1</v>
@@ -9704,13 +9708,13 @@
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="G8" s="28">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
@@ -9718,7 +9722,7 @@
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="O8" s="28">
         <v>0.1</v>
@@ -9743,10 +9747,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="28">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -9754,7 +9758,7 @@
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="O9" s="28">
         <v>0.1</v>
@@ -9779,10 +9783,10 @@
         <v>-0.5</v>
       </c>
       <c r="G10" s="28">
-        <v>2.5</v>
+        <v>0.25</v>
       </c>
       <c r="H10" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -9790,7 +9794,7 @@
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="O10" s="28">
         <v>0.1</v>
@@ -9815,10 +9819,10 @@
         <v>-0.5</v>
       </c>
       <c r="G11" s="28">
-        <v>2.5</v>
+        <v>0.25</v>
       </c>
       <c r="H11" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
@@ -9826,7 +9830,7 @@
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="O11" s="28">
         <v>0.1</v>
@@ -9846,7 +9850,7 @@
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
@@ -9868,7 +9872,7 @@
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
@@ -9890,7 +9894,7 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -9920,7 +9924,7 @@
         <v>0.33</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -9933,7 +9937,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -9942,7 +9946,7 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
@@ -9955,7 +9959,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -9964,7 +9968,7 @@
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
@@ -9977,7 +9981,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -9986,12 +9990,12 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -10000,7 +10004,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
   </sheetData>
@@ -10275,7 +10279,7 @@
         <v>16.023499999999999</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>1029</v>
@@ -10302,7 +10306,7 @@
         <v>14.716100000000001</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="N10" s="28" t="s">
         <v>1026</v>
@@ -10570,7 +10574,7 @@
         <v>0.87390000000000001</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="N20" t="s">
         <v>1133</v>
@@ -10650,7 +10654,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N27" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="O27" s="28">
         <v>0</v>
@@ -10661,7 +10665,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="O28" s="28">
         <v>0</v>
@@ -10683,7 +10687,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="O30" s="28">
         <v>0</v>
@@ -10694,7 +10698,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="O31" s="28">
         <v>0</v>
@@ -10705,7 +10709,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="O32" s="28">
         <v>0</v>
@@ -10716,7 +10720,7 @@
     </row>
     <row r="33" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="O33" s="28">
         <v>0</v>
@@ -56813,7 +56817,7 @@
         <v>884</v>
       </c>
       <c r="N60" s="28" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="O60" s="28">
         <v>0</v>
@@ -56840,7 +56844,7 @@
         <v>1149</v>
       </c>
       <c r="N61" s="28" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="O61" s="28">
         <v>0</v>

</xml_diff>

<commit_message>
Daily Updates July 2
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,16 +16,17 @@
     <sheet name="N2" sheetId="13" r:id="rId7"/>
     <sheet name="N2mR" sheetId="20" r:id="rId8"/>
     <sheet name="N2mD" sheetId="17" r:id="rId9"/>
-    <sheet name="lacOP" sheetId="16" r:id="rId10"/>
-    <sheet name="N2lacZ" sheetId="15" r:id="rId11"/>
-    <sheet name="N3" sheetId="14" r:id="rId12"/>
-    <sheet name="N3mR" sheetId="19" r:id="rId13"/>
-    <sheet name="PTS" sheetId="8" r:id="rId14"/>
-    <sheet name="Sheet6" sheetId="10" r:id="rId15"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId16"/>
-    <sheet name="Sheet7" sheetId="11" r:id="rId17"/>
-    <sheet name="EcoliCCM" sheetId="18" r:id="rId18"/>
-    <sheet name="testN2m" sheetId="12" r:id="rId19"/>
+    <sheet name="N2mC" sheetId="21" r:id="rId10"/>
+    <sheet name="lacOP" sheetId="16" r:id="rId11"/>
+    <sheet name="N2lacZ" sheetId="15" r:id="rId12"/>
+    <sheet name="N3" sheetId="14" r:id="rId13"/>
+    <sheet name="N3mR" sheetId="19" r:id="rId14"/>
+    <sheet name="PTS" sheetId="8" r:id="rId15"/>
+    <sheet name="Sheet6" sheetId="10" r:id="rId16"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId17"/>
+    <sheet name="Sheet7" sheetId="11" r:id="rId18"/>
+    <sheet name="EcoliCCM" sheetId="18" r:id="rId19"/>
+    <sheet name="testN2m" sheetId="12" r:id="rId20"/>
   </sheets>
   <calcPr calcId="145621"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="1270">
   <si>
     <t>Name</t>
   </si>
@@ -3747,15 +3748,6 @@
   </si>
   <si>
     <t>Bex</t>
-  </si>
-  <si>
-    <t>[c] : D ---&gt; A</t>
-  </si>
-  <si>
-    <t>[c] : P + E ---&gt; C + D</t>
-  </si>
-  <si>
-    <t>20 B[c] ---&gt; Biomass[c]</t>
   </si>
   <si>
     <t>Biomass[c] ---&gt;</t>
@@ -4028,7 +4020,25 @@
     <t>v6</t>
   </si>
   <si>
-    <t>50</t>
+    <t>[c] : A &lt;==&gt; D</t>
+  </si>
+  <si>
+    <t>[c] : C + D &lt;==&gt; P + E</t>
+  </si>
+  <si>
+    <t>&lt;==&gt; E[e]</t>
+  </si>
+  <si>
+    <t>&lt;==&gt; D[e]</t>
+  </si>
+  <si>
+    <t>D[e] &lt;==&gt; D[c]</t>
+  </si>
+  <si>
+    <t>E[e] &lt;==&gt; E[c]</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -5643,6 +5653,587 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>818</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>828</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B2" s="28">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="s">
+        <v>1190</v>
+      </c>
+      <c r="O2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G3" s="28">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28" t="s">
+        <v>1122</v>
+      </c>
+      <c r="O3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G4" s="28">
+        <v>20</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G5" s="28">
+        <v>20</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28" t="s">
+        <v>1123</v>
+      </c>
+      <c r="O5" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B6" s="28">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
+        <v>10</v>
+      </c>
+      <c r="G6" s="28">
+        <v>-40</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>1263</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O6" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P6" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G7" s="28">
+        <v>20</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
+        <v>1124</v>
+      </c>
+      <c r="O7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G8" s="28">
+        <v>20</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28">
+        <v>10</v>
+      </c>
+      <c r="G9" s="28">
+        <v>-20</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>1264</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>5</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>1268</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B12" s="28">
+        <v>0</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>1267</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B16" s="28">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6057,7 +6648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
@@ -6580,7 +7171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -6979,7 +7570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
@@ -7041,7 +7632,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -7105,7 +7696,7 @@
     </row>
     <row r="4" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="B4" s="28">
         <v>0</v>
@@ -7141,7 +7732,7 @@
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="B5" s="28">
         <v>0</v>
@@ -7177,7 +7768,7 @@
     </row>
     <row r="6" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="B6" s="28">
         <v>0</v>
@@ -7213,7 +7804,7 @@
     </row>
     <row r="7" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="B7" s="28">
         <v>0</v>
@@ -7249,7 +7840,7 @@
     </row>
     <row r="8" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="B8" s="28">
         <v>0</v>
@@ -7285,7 +7876,7 @@
     </row>
     <row r="9" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="B9" s="28">
         <v>0</v>
@@ -7307,11 +7898,11 @@
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="28" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>1227</v>
@@ -7325,7 +7916,7 @@
     </row>
     <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="B10" s="28">
         <v>0</v>
@@ -7361,7 +7952,7 @@
     </row>
     <row r="11" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B11" s="28">
         <v>0</v>
@@ -7397,7 +7988,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="B12" s="28">
         <v>0</v>
@@ -7425,7 +8016,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="B13" s="28">
         <v>0</v>
@@ -7453,7 +8044,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="B14" s="28">
         <v>0</v>
@@ -7498,7 +8089,7 @@
         <v>0.33</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -7611,7 +8202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P60"/>
   <sheetViews>
@@ -9194,7 +9785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -9435,7 +10026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
@@ -9921,7 +10512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -10266,7 +10857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
@@ -10989,7 +11580,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P128"/>
   <sheetViews>
@@ -13398,224 +14207,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -57910,7 +58501,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58047,7 +58638,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="B4" s="28">
         <v>0</v>
@@ -58085,7 +58676,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="B5" s="28">
         <v>0</v>
@@ -58123,7 +58714,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="B6" s="28">
         <v>0</v>
@@ -58134,13 +58725,13 @@
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="G6" s="28">
-        <v>-40</v>
+        <v>40</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -58161,7 +58752,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="B7" s="28">
         <v>0</v>
@@ -58199,7 +58790,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="B8" s="28">
         <v>0</v>
@@ -58207,37 +58798,31 @@
       <c r="C8" s="28">
         <v>3000</v>
       </c>
-      <c r="D8" s="28">
-        <v>30</v>
-      </c>
+      <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28">
         <v>-8</v>
       </c>
       <c r="G8" s="28">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>1117</v>
       </c>
-      <c r="I8" s="28" t="s">
-        <v>1125</v>
-      </c>
+      <c r="I8" s="28"/>
       <c r="J8" s="1"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28" t="s">
         <v>1077</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>1266</v>
-      </c>
+      <c r="M8" s="1"/>
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="B9" s="28">
         <v>0</v>
@@ -58245,27 +58830,33 @@
       <c r="C9" s="28">
         <v>3000</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="28">
+        <v>15</v>
+      </c>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="G9" s="28">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>1118</v>
       </c>
-      <c r="J9" s="28"/>
+      <c r="I9" t="s">
+        <v>1124</v>
+      </c>
       <c r="K9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="M9" s="1" t="s">
+        <v>1269</v>
+      </c>
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
       <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="B10" s="28">
         <v>0</v>
@@ -58295,7 +58886,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="B11" s="28">
         <v>0</v>
@@ -58312,7 +58903,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
@@ -58325,7 +58916,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="B12" s="28">
         <v>0</v>
@@ -58342,7 +58933,7 @@
         <v>0.33</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
@@ -58385,7 +58976,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="B14" s="28">
         <v>0</v>
@@ -58402,7 +58993,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -58432,7 +59023,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -58445,7 +59036,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -58460,7 +59051,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
@@ -58488,7 +59079,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
@@ -58509,7 +59100,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58570,8 +59161,14 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="28" t="s">
         <v>1206</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
       </c>
       <c r="H2" t="s">
         <v>1207</v>
@@ -58631,13 +59228,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>1054</v>
+        <v>1257</v>
       </c>
       <c r="B4" s="28">
         <v>0</v>
       </c>
       <c r="C4" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -58669,13 +59266,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>764</v>
+        <v>1258</v>
       </c>
       <c r="B5" s="28">
         <v>0</v>
       </c>
       <c r="C5" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
@@ -58707,24 +59304,24 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>1055</v>
+        <v>1259</v>
       </c>
       <c r="B6" s="28">
         <v>0</v>
       </c>
       <c r="C6" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G6" s="28">
-        <v>40</v>
+        <v>-40</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>1231</v>
+        <v>1263</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
@@ -58745,13 +59342,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>1056</v>
+        <v>1260</v>
       </c>
       <c r="B7" s="28">
         <v>0</v>
       </c>
       <c r="C7" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
@@ -58783,13 +59380,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>1059</v>
+        <v>1261</v>
       </c>
       <c r="B8" s="28">
         <v>0</v>
       </c>
       <c r="C8" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -58815,24 +59412,24 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>1058</v>
+        <v>1262</v>
       </c>
       <c r="B9" s="28">
         <v>0</v>
       </c>
       <c r="C9" s="28">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G9" s="28">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>1232</v>
+        <v>1264</v>
       </c>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
@@ -58845,7 +59442,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="B10" s="28">
         <v>0</v>
@@ -58875,7 +59472,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="B11" s="28">
         <v>0</v>
@@ -58892,17 +59489,17 @@
         <v>2.5</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="28">
         <v>0</v>
       </c>
       <c r="F12">
@@ -58912,17 +59509,17 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1235</v>
+      <c r="A13" s="28" t="s">
+        <v>1232</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="28">
         <v>0</v>
       </c>
       <c r="F13">
@@ -58932,11 +59529,11 @@
         <v>0.33</v>
       </c>
       <c r="H13" t="s">
-        <v>1233</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="28" t="s">
         <v>1201</v>
       </c>
       <c r="B14" s="28">
@@ -58976,23 +59573,35 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1236</v>
+      <c r="A16" s="28" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="28" t="s">
         <v>1204</v>
       </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0</v>
+      </c>
       <c r="H17" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dailu Updates Jul;y 29
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="1257">
   <si>
     <t>Name</t>
   </si>
@@ -3808,6 +3808,27 @@
   </si>
   <si>
     <t>[c] : M  + N ---&gt; biomass</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>.1</t>
   </si>
 </sst>
 </file>
@@ -57673,11 +57694,12 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
@@ -57810,7 +57832,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>1054</v>
+        <v>1250</v>
       </c>
       <c r="B4" s="28">
         <v>0</v>
@@ -57848,7 +57870,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>764</v>
+        <v>1251</v>
       </c>
       <c r="B5" s="28">
         <v>0</v>
@@ -57886,7 +57908,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>1055</v>
+        <v>1252</v>
       </c>
       <c r="B6" s="28">
         <v>0</v>
@@ -57897,10 +57919,10 @@
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28">
-        <v>10</v>
+        <v>-8</v>
       </c>
       <c r="G6" s="28">
-        <v>-40</v>
+        <v>40</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>1241</v>
@@ -57924,7 +57946,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>1056</v>
+        <v>1253</v>
       </c>
       <c r="B7" s="28">
         <v>0</v>
@@ -57962,7 +57984,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>1059</v>
+        <v>1254</v>
       </c>
       <c r="B8" s="28">
         <v>0</v>
@@ -57970,7 +57992,9 @@
       <c r="C8" s="28">
         <v>3000</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="28">
+        <v>15</v>
+      </c>
       <c r="E8" s="28"/>
       <c r="F8" s="28">
         <v>-8</v>
@@ -57982,19 +58006,23 @@
         <v>1117</v>
       </c>
       <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="J8" s="28" t="s">
+        <v>1125</v>
+      </c>
       <c r="K8" s="28"/>
       <c r="L8" s="28" t="s">
         <v>1077</v>
       </c>
-      <c r="M8" s="28"/>
+      <c r="M8" s="1" t="s">
+        <v>1256</v>
+      </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>1058</v>
+        <v>1255</v>
       </c>
       <c r="B9" s="28">
         <v>0</v>
@@ -58005,18 +58033,17 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G9" s="28">
         <v>10</v>
-      </c>
-      <c r="G9" s="28">
-        <v>-10</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>1118</v>
       </c>
-      <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
       <c r="P9" s="28"/>

</xml_diff>

<commit_message>
Branch Closing commit 1
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,26 +14,27 @@
     <sheet name="MN 1" sheetId="6" r:id="rId5"/>
     <sheet name="SN 1" sheetId="7" r:id="rId6"/>
     <sheet name="N2" sheetId="13" r:id="rId7"/>
-    <sheet name="N2mR" sheetId="20" r:id="rId8"/>
-    <sheet name="N2mD" sheetId="17" r:id="rId9"/>
+    <sheet name="N2m" sheetId="22" r:id="rId8"/>
+    <sheet name="N2mR" sheetId="20" r:id="rId9"/>
     <sheet name="N2mC" sheetId="21" r:id="rId10"/>
-    <sheet name="lacOP" sheetId="16" r:id="rId11"/>
-    <sheet name="N2lacZ" sheetId="15" r:id="rId12"/>
-    <sheet name="N3" sheetId="14" r:id="rId13"/>
-    <sheet name="N3mR" sheetId="19" r:id="rId14"/>
-    <sheet name="PTS" sheetId="8" r:id="rId15"/>
-    <sheet name="Sheet6" sheetId="10" r:id="rId16"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId17"/>
-    <sheet name="Sheet7" sheetId="11" r:id="rId18"/>
-    <sheet name="EcoliCCM" sheetId="18" r:id="rId19"/>
-    <sheet name="testN2m" sheetId="12" r:id="rId20"/>
+    <sheet name="N2mD" sheetId="17" r:id="rId11"/>
+    <sheet name="lacOP" sheetId="16" r:id="rId12"/>
+    <sheet name="N2lacZ" sheetId="15" r:id="rId13"/>
+    <sheet name="N3" sheetId="14" r:id="rId14"/>
+    <sheet name="N3mD" sheetId="19" r:id="rId15"/>
+    <sheet name="PTS" sheetId="8" r:id="rId16"/>
+    <sheet name="Sheet6" sheetId="10" r:id="rId17"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId18"/>
+    <sheet name="Sheet7" sheetId="11" r:id="rId19"/>
+    <sheet name="EcoliCCM" sheetId="18" r:id="rId20"/>
+    <sheet name="testN2m" sheetId="12" r:id="rId21"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2382" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="1268">
   <si>
     <t>Name</t>
   </si>
@@ -6220,6 +6221,521 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>818</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>828</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="s">
+        <v>1190</v>
+      </c>
+      <c r="O2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G3" s="28">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28" t="s">
+        <v>1122</v>
+      </c>
+      <c r="O3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G4" s="28">
+        <v>20</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G5" s="28">
+        <v>20</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28" t="s">
+        <v>1123</v>
+      </c>
+      <c r="O5" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B6" s="28">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
+        <v>10</v>
+      </c>
+      <c r="G6" s="28">
+        <v>-40</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>1261</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O6" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P6" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G7" s="28">
+        <v>20</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
+        <v>1124</v>
+      </c>
+      <c r="O7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G8" s="28">
+        <v>20</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28">
+        <v>10</v>
+      </c>
+      <c r="G9" s="28">
+        <v>-10</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>1262</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>5</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G11" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>-0.5</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>-0.5</v>
+      </c>
+      <c r="G13">
+        <v>0.33</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6634,7 +7150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
@@ -7157,7 +7673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -7556,11 +8072,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -8184,7 +8700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P60"/>
   <sheetViews>
@@ -9767,7 +10283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -10008,7 +10524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
@@ -10494,7 +11010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
@@ -10839,7 +11355,225 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
@@ -11562,225 +12296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P128"/>
   <sheetViews>
@@ -58483,7 +58999,600 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>818</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>828</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B2" s="28">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28">
+        <v>0</v>
+      </c>
+      <c r="G2" s="28">
+        <v>5</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>1207</v>
+      </c>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="s">
+        <v>1190</v>
+      </c>
+      <c r="O2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P2" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B3" s="28">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G3" s="28">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28" t="s">
+        <v>1122</v>
+      </c>
+      <c r="O3" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P3" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G4" s="28">
+        <v>20</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>1187</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28" t="s">
+        <v>1121</v>
+      </c>
+      <c r="O4" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P4" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G5" s="28">
+        <v>20</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28" t="s">
+        <v>1123</v>
+      </c>
+      <c r="O5" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B6" s="28">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G6" s="28">
+        <v>40</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>1238</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O6" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P6" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B7" s="28">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G7" s="28">
+        <v>20</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28" t="s">
+        <v>1124</v>
+      </c>
+      <c r="O7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="P7" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G8" s="28">
+        <v>30</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>1117</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28">
+        <v>-8</v>
+      </c>
+      <c r="G9" s="28">
+        <v>10</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>5</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>1189</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B12" s="28">
+        <v>0</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>1239</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B14" s="28">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>1234</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B15" s="28">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>1231</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B16" s="28">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G16" s="28">
+        <v>0</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>1237</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28">
+        <v>-0.5</v>
+      </c>
+      <c r="G17" s="28">
+        <v>0</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59075,519 +60184,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>565</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>728</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>731</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>729</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>730</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>830</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>818</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>608</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>609</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>654</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>656</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>657</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>726</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>828</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>1206</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1207</v>
-      </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28" t="s">
-        <v>1190</v>
-      </c>
-      <c r="O2" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P2" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>1057</v>
-      </c>
-      <c r="B3" s="28">
-        <v>0</v>
-      </c>
-      <c r="C3" s="28">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28">
-        <v>-8</v>
-      </c>
-      <c r="G3" s="28">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28" t="s">
-        <v>1122</v>
-      </c>
-      <c r="O3" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P3" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B4" s="28">
-        <v>0</v>
-      </c>
-      <c r="C4" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28">
-        <v>-8</v>
-      </c>
-      <c r="G4" s="28">
-        <v>20</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>1187</v>
-      </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28" t="s">
-        <v>1121</v>
-      </c>
-      <c r="O4" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P4" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B5" s="28">
-        <v>0</v>
-      </c>
-      <c r="C5" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28">
-        <v>-8</v>
-      </c>
-      <c r="G5" s="28">
-        <v>20</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>1188</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28" t="s">
-        <v>1123</v>
-      </c>
-      <c r="O5" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P5" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B6" s="28">
-        <v>0</v>
-      </c>
-      <c r="C6" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28">
-        <v>10</v>
-      </c>
-      <c r="G6" s="28">
-        <v>-40</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>1261</v>
-      </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28" t="s">
-        <v>1125</v>
-      </c>
-      <c r="O6" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P6" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B7" s="28">
-        <v>0</v>
-      </c>
-      <c r="C7" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28">
-        <v>-8</v>
-      </c>
-      <c r="G7" s="28">
-        <v>20</v>
-      </c>
-      <c r="H7" s="28" t="s">
-        <v>1191</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28" t="s">
-        <v>667</v>
-      </c>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28" t="s">
-        <v>1124</v>
-      </c>
-      <c r="O7" s="28">
-        <v>0.1</v>
-      </c>
-      <c r="P7" s="28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>1259</v>
-      </c>
-      <c r="B8" s="28">
-        <v>0</v>
-      </c>
-      <c r="C8" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28">
-        <v>-8</v>
-      </c>
-      <c r="G8" s="28">
-        <v>20</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>1117</v>
-      </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28" t="s">
-        <v>1077</v>
-      </c>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B9" s="28">
-        <v>0</v>
-      </c>
-      <c r="C9" s="28">
-        <v>3000</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28">
-        <v>10</v>
-      </c>
-      <c r="G9" s="28">
-        <v>-10</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>1262</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B10" s="28">
-        <v>0</v>
-      </c>
-      <c r="C10" s="28">
-        <v>0</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G10" s="28">
-        <v>5</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>1189</v>
-      </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B11" s="28">
-        <v>0</v>
-      </c>
-      <c r="C11" s="28">
-        <v>0</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G11" s="28">
-        <v>2.5</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="28">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>-0.5</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>1232</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" s="28">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>-0.5</v>
-      </c>
-      <c r="G13">
-        <v>0.33</v>
-      </c>
-      <c r="H13" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B14" s="28">
-        <v>0</v>
-      </c>
-      <c r="C14" s="28">
-        <v>0</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1202</v>
-      </c>
-      <c r="B15" s="28">
-        <v>0</v>
-      </c>
-      <c r="C15" s="28">
-        <v>0</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28">
-        <v>-0.5</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="28">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>1204</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="28">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Works till calculation of FBA fluxes
</commit_message>
<xml_diff>
--- a/KineticModel/test.xlsx
+++ b/KineticModel/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4665" windowWidth="16275" windowHeight="3180" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="4725" windowWidth="16275" windowHeight="3120" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6223,14 +6223,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -59591,7 +59591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>